<commit_message>
Criado os arquivos de trabalho
</commit_message>
<xml_diff>
--- a/Documentacao/Lista de tarefas.xlsx
+++ b/Documentacao/Lista de tarefas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valentino_pascual\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valentino_pascual\Desktop\F1_Novo\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>Mamedes</t>
   </si>
@@ -213,17 +213,39 @@
   </si>
   <si>
     <t>Audio</t>
+  </si>
+  <si>
+    <t>Inicialização do projeto</t>
+  </si>
+  <si>
+    <t>index.html(front)</t>
+  </si>
+  <si>
+    <t>style.css(front)</t>
+  </si>
+  <si>
+    <t>f1_class.js</t>
+  </si>
+  <si>
+    <t>f1_main.js(backend)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -418,12 +440,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -431,25 +453,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -457,14 +479,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2997,15 +3020,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F27"/>
+  <dimension ref="B1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
@@ -3277,6 +3300,31 @@
       </c>
       <c r="F27" s="17"/>
     </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="28" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>